<commit_message>
Update test tab call to use new named path to request functionality.
</commit_message>
<xml_diff>
--- a/example_usage/suites/jsonExample.xlsx
+++ b/example_usage/suites/jsonExample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felala\Documents\demo_back\TcdsIntegration\example_usage\suites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mposlus1\Documents\GitHub\codeless\example_usage\suites\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B5C43C-B050-48D9-9075-8B8EB9A60D6D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="24600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c-demo_ui" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>key</t>
   </si>
@@ -102,9 +103,6 @@
     <t>Path to the ie webdriver to use for this machine. Installed under &lt;INSTALL_DIR&gt;/webdrivers/&lt;OS&gt; by default. Windows only, no other valid settings.</t>
   </si>
   <si>
-    <t>GET</t>
-  </si>
-  <si>
     <t>TRUE</t>
   </si>
   <si>
@@ -165,9 +163,6 @@
     <t>goto</t>
   </si>
   <si>
-    <t>sample.api.create</t>
-  </si>
-  <si>
     <t>close browser</t>
   </si>
   <si>
@@ -237,19 +232,19 @@
     <t>{{imdbhome}}</t>
   </si>
   <si>
-    <t>endpoint::host::{{serviceCall.omdbhost}}::path::{{serviceCall.omdbpath}}</t>
-  </si>
-  <si>
     <t>{{almId}}</t>
   </si>
   <si>
     <t>TestData::tcds</t>
+  </si>
+  <si>
+    <t>omdb.Wall-E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -633,22 +628,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="4"/>
+    <col min="3" max="3" width="62.42578125" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -659,7 +654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -670,18 +665,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -692,7 +687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
@@ -703,7 +698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
@@ -714,163 +709,163 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="6" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="6" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="8" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="11"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="11"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="B22" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="11"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="11"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="11"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="11"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="8" t="s">
+      <c r="B23" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="11"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="8" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="11"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="8" t="s">
+      <c r="B24" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -880,25 +875,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="3" width="33.77734375" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="65.33203125" customWidth="1"/>
-    <col min="6" max="6" width="44.33203125" customWidth="1"/>
-    <col min="7" max="7" width="45.109375" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="65.28515625" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" customWidth="1"/>
+    <col min="7" max="7" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -922,7 +917,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
@@ -932,78 +927,74 @@
       <c r="C2" s="1"/>
       <c r="D2" s="10"/>
       <c r="E2" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>25</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>49</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F3" s="10"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="F5" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G6" s="2"/>
     </row>

</xml_diff>